<commit_message>
sector summaries and direct indirect emissions
</commit_message>
<xml_diff>
--- a/Results/Plots/captions.xlsx
+++ b/Results/Plots/captions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>Global greenhouse gas emissions and their sources</t>
   </si>
   <si>
-    <t>The stacked bar on the left indicates total global greenhouse gas emissions in 2018, split by sectors based on direct (scope 1) emissions accounting. The arrows shown next to the electricity and heat sector depict the reallocation of these emissions to final sectors as indirect (scope 2) emissions. This increases the contribution to global emissions from the industry and buildings sector (central stacked bar). The stacked bar on the far right indicates the shares of subsectors in global emissions when indirect emissions are included.</t>
-  </si>
-  <si>
     <t>Total global emissions by highest emitting subsectors</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>Reproduced from Hong et al (Hong et al 2021).The indicated growth rates are averaged across the years 2010-2017. In contrast to other kaya figures, here we show total GHG emissions for the AFOLU sector.</t>
+  </si>
+  <si>
+    <t>The stacked bar on the left indicates total global greenhouse gas emissions in 2019, split by sectors based on direct (scope 1) emissions accounting. The arrows shown next to the electricity and heat sector depict the reallocation of these emissions to final sectors as indirect (scope 2) emissions. This increases the contribution to global emissions from the industry and buildings sector (central stacked bar). This reallocation does not imply full lifecycle emissions – see Annex B {A.B.8} for more details. The stacked bar on the far right indicates the shares of subsectors in global emissions when indirect emissions are included. GHG emissions are reported in GtCO2-eq, based on global warming potentials with a 100-year time horizon (GWP-100) from the IPCC Sixth Assessment Working Group 1 Report.</t>
   </si>
 </sst>
 </file>
@@ -498,13 +498,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -515,7 +515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -537,7 +537,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -545,10 +545,10 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -559,151 +559,151 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated and added regions_countries
</commit_message>
<xml_diff>
--- a/Results/Plots/captions.xlsx
+++ b/Results/Plots/captions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>gases</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>CO2 from fossil fuel combustion and industrial processes (FFI); CO2 from Land use, land use change and forestry (CO2 LULUCF); methane (CH4); nitrous oxide (N2O); fluorinated gases (F-gases). CO2 LULUCF emissions are net and include gross removals as well as emissions. F-gas emissions do not include Montreal gases (CFCs, HCFCs) which reached a peak in the 1990s but have since declined. Panel a: Aggregate GHG emission trends by groups of gases reported in GtCO2-eq converted based on global warming potentials with a 100-year time horizon (GWP-100) from the IPCC Sixth Assessment Report Working Group 1 (REF Chapter 7). Panel b: Waterfall diagrams juxtaposing GHG emissions for the most recent year 2019 in CO2 equivalent units using GWP-100  values from the IPCC’s Sixth, Fifth and Second Assessment Reports, respectively. Error bars show the associated uncertainties at a 90% confidence interval. Panel c: Individual trends in CO2-FFI, CO2-FOLU, CH4 and N2O emissions in (original) mass units 10 (Gt yr-1) for the period 1990–2019, normalised relative to 1 in 1990. Note the different scale for F-gas emissions compared to other gases, highlighting its very rapid growth from a low base.</t>
+  </si>
+  <si>
+    <t>regions_countries</t>
+  </si>
+  <si>
+    <t>Change in regional GHGs from multiple perspectives and their underlying drivers</t>
+  </si>
+  <si>
+    <t>Panel a: Regional GHG emission trends (in GtCO2eq yr-1) for the time period 1990-2019. GHG emissions from international aviation (AIR) and shipping (SEA) are not assigned to individual countries and shown separately. Panels b and c: Changes in GHG emissions for largest emitters (75% of global emissions) for the post-AR5 reporting period 2010-2019 in relative (% annual change) and absolute terms (GtCO2eq). Panels d and e: GHG emissions per capita and per GDP in 2019 for the largest emitters (75% of global emissions). GDP estimated using constant international purchasing power parity (USD 2017). Emissions are converted into CO2-equivalents based on global warming potentials with a 100 year time horizon (GWP-100) from the IPCC Sixth Assessment Report. The yellow dots represent the emissions data according to the national inventories reported by the Annex I countries of the Kyoto Protocol to the UNFCCC (Gütschow et al., 2021; Louise Jeffery et al., 2018).  LULUCF CO2 emissions are included in panel a, based on the average of three bookkeeping models (see data explanation in section 2.2 introduction), but are excluded in panels b to e due to a lack of regional resolution.</t>
   </si>
 </sst>
 </file>
@@ -514,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,181 +577,192 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>